<commit_message>
Updated 8am 5/20/17 PH Time
</commit_message>
<xml_diff>
--- a/resources/Authorization.xlsx
+++ b/resources/Authorization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780" tabRatio="917" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780" tabRatio="917" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorizationASSIGNTO" sheetId="1" r:id="rId1"/>
@@ -15,19 +15,18 @@
     <sheet name="AuthorizationAddComment" sheetId="6" r:id="rId6"/>
     <sheet name="AuthorizationResponseAuthz1" sheetId="7" r:id="rId7"/>
     <sheet name="AuthorizationResponseAuthz2" sheetId="13" r:id="rId8"/>
-    <sheet name="AuthorizationSaveRes" sheetId="8" r:id="rId9"/>
-    <sheet name="AuthorizationSendAuths2" sheetId="9" r:id="rId10"/>
-    <sheet name="authz3" sheetId="10" r:id="rId11"/>
-    <sheet name="authz4" sheetId="14" r:id="rId12"/>
-    <sheet name="AuthorizationSaveResponseAuthz" sheetId="11" r:id="rId13"/>
-    <sheet name="AuthorizationApproved" sheetId="12" r:id="rId14"/>
+    <sheet name="AuthorizationSendAuths2" sheetId="9" r:id="rId9"/>
+    <sheet name="authz3" sheetId="10" r:id="rId10"/>
+    <sheet name="authz4" sheetId="14" r:id="rId11"/>
+    <sheet name="AuthorizationSaveResponseAuthz" sheetId="11" r:id="rId12"/>
+    <sheet name="AuthorizationApproved" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -276,6 +275,12 @@
   </si>
   <si>
     <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]/md-select-menu//md-option[1]</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="vm.receiveAuthResponse(exchange, auth, $event)" and @aria-hidden="false"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -647,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -912,250 +917,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" ht="11.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="60">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="27" customHeight="1">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="G8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="100.5" customHeight="1">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -1194,7 +961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1215,7 +982,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="150">
+    <row r="10" spans="1:8" ht="75">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1380,12 +1147,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1482,21 +1249,167 @@
       </c>
       <c r="H4" s="10"/>
     </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="49.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
@@ -1767,7 +1680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -2216,7 +2129,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2449,7 +2362,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2758,7 +2671,7 @@
         <v>17</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2811,7 +2724,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3122,7 +3035,7 @@
         <v>17</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3172,14 +3085,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3449,8 +3363,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="B14" s="3"/>
+    <row r="14" spans="1:8" ht="45">
+      <c r="B14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3459,10 +3408,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3501,7 +3450,7 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -3522,7 +3471,7 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -3538,17 +3487,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="48" customHeight="1">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
       <c r="E4">
         <v>1</v>
       </c>
@@ -3561,120 +3509,266 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="48" customHeight="1">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="35.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" customHeight="1">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="D14" s="4"/>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A7" t="s">
+    <row r="15" spans="1:8" ht="106.5" customHeight="1">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" customHeight="1">
-      <c r="A8" t="s">
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="106.5" customHeight="1">
-      <c r="A10" t="s">
+      <c r="D17" s="6"/>
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
         <v>5</v>
       </c>
     </row>
@@ -3685,10 +3779,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15"/>
@@ -3724,32 +3818,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="46.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="46.5" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -3766,15 +3850,35 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
         <v>3</v>
       </c>
     </row>
@@ -3785,15 +3889,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="60">
@@ -3822,7 +3927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="27" customHeight="1">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3841,13 +3946,12 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -3863,17 +3967,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="62.25" customHeight="1">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="4"/>
       <c r="E4">
         <v>1</v>
       </c>
@@ -3886,52 +3990,52 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="34.5" customHeight="1">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="36.75" customHeight="1">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4"/>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="42.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -3944,118 +4048,77 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="36.75" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
       <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="100.5" customHeight="1">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="64.5" customHeight="1">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="72" customHeight="1">
-      <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="48" customHeight="1">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated as of 5/24/17
</commit_message>
<xml_diff>
--- a/resources/Authorization.xlsx
+++ b/resources/Authorization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780" tabRatio="917" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780" tabRatio="917" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorizationASSIGNTO" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -1149,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1248,151 +1248,6 @@
         <v>3</v>
       </c>
       <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1684,12 +1539,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
@@ -1839,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -1874,7 +1730,7 @@
         <v>31</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="47.25" customHeight="1">
@@ -1928,7 +1784,7 @@
         <v>31</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3781,7 +3637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD24"/>
     </sheetView>
   </sheetViews>
@@ -3891,8 +3747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4119,6 +3975,9 @@
         <v>31</v>
       </c>
       <c r="D11" s="6"/>
+      <c r="G11">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>